<commit_message>
Added DCF Model for NVDA - need to add Street Predictions from Brokers
</commit_message>
<xml_diff>
--- a/Google.xlsx
+++ b/Google.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gus-c\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF94064E-90D0-46C1-B01E-EA37CB5E94E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39083950-E109-406D-9E54-272F5173EEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{FC0C9081-A75D-4766-A729-B939A9D07BD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Model" sheetId="2" r:id="rId2"/>
-    <sheet name="teste" sheetId="4" r:id="rId3"/>
-    <sheet name="Formulas" sheetId="3" r:id="rId4"/>
+    <sheet name="Formulas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Price</t>
   </si>
@@ -177,9 +176,6 @@
   </si>
   <si>
     <t>Cloud Growth</t>
-  </si>
-  <si>
-    <t>dfdfdf</t>
   </si>
 </sst>
 </file>
@@ -1419,30 +1415,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE59A32-6D1E-4ADE-A21B-88E474939479}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8A4E8D-667C-4737-A22D-97EBDDE12299}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>

</xml_diff>